<commit_message>
Design Response For When There Are No Cases Left For The Day
</commit_message>
<xml_diff>
--- a/excel/cases.xlsx
+++ b/excel/cases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Program Files\Programs\Web Dev Related Stuff\Web Dev\Projects\Web Apllication Competition\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Program Files\Programs\Web Dev Related Stuff\Web Dev\Projects\EvaTion\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B34A293-842C-4AFE-B1B6-A4A0A3A76378}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDAC64A7-B376-4037-A1C8-0A0A86E57BC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -111,9 +111,6 @@
     <t>Seorang staff menemukan narkotika didalam kabinet obat-obatan farmasi lain dan langsung melaporkannya.</t>
   </si>
   <si>
-    <t xml:space="preserve">Saat sedang melakukan pengecekan, sebuah narkotika yg berada pada tablet obat tanpa label ditemukan dalam sebuah farmasi. </t>
-  </si>
-  <si>
     <t>Kasus ini diarahkan kepada farmasi. Seorang pecandu melaporkan dirinya sendiri dan memberi tau siapa pengedarnya, setelah ditangkap pengedar mengaku bekerja di perusahaan perdagangan yang memberikan sedikit narkotika kepada staff yang bekerja pada narkotika itu, dengan cara membeli lebih dari permintaan farmasi.</t>
   </si>
   <si>
@@ -232,6 +229,9 @@
   </si>
   <si>
     <t>Menurut UU no.35 tahun 2009, pasal 55, 112, 114, 127, dan 134 ayat (1). Pecandu bersalah dan akan direhabilitas sesuai pasal 56.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saat sedang melakukan pengecekan, sebuah narkotika yang berada pada tablet obat tanpa label ditemukan dalam sebuah farmasi. </t>
   </si>
 </sst>
 </file>
@@ -634,7 +634,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.8984375" defaultRowHeight="18"/>
@@ -678,7 +678,7 @@
         <v>18</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>10</v>
@@ -698,7 +698,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>11</v>
@@ -718,7 +718,7 @@
         <v>20</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>12</v>
@@ -738,7 +738,7 @@
         <v>21</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>13</v>
@@ -758,7 +758,7 @@
         <v>22</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>12</v>
@@ -778,7 +778,7 @@
         <v>23</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>13</v>
@@ -798,7 +798,7 @@
         <v>24</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>12</v>
@@ -818,7 +818,7 @@
         <v>26</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>13</v>
@@ -838,7 +838,7 @@
         <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>12</v>
@@ -858,7 +858,7 @@
         <v>6</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>13</v>
@@ -878,7 +878,7 @@
         <v>27</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>12</v>
@@ -895,10 +895,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>13</v>
@@ -915,10 +915,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>12</v>
@@ -935,10 +935,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>13</v>
@@ -955,10 +955,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>12</v>
@@ -975,10 +975,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>13</v>
@@ -998,7 +998,7 @@
         <v>7</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>12</v>
@@ -1015,10 +1015,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>13</v>
@@ -1035,10 +1035,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>12</v>
@@ -1055,10 +1055,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>13</v>
@@ -1075,10 +1075,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>12</v>
@@ -1095,10 +1095,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>12</v>
@@ -1115,10 +1115,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>13</v>
@@ -1135,10 +1135,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>12</v>
@@ -1155,10 +1155,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>12</v>
@@ -1175,7 +1175,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>8</v>
@@ -1198,7 +1198,7 @@
         <v>9</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>14</v>
@@ -1215,10 +1215,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>15</v>
@@ -1235,10 +1235,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>16</v>
@@ -1255,10 +1255,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Some Text Changes In Cases, Z-Index For Sidebar And Modals, Active Class For Links In Sidebar, Design For Setting Page, Some Adjustment In SCSS Code & Created Reset Data and Logout In Setting Page
</commit_message>
<xml_diff>
--- a/excel/cases.xlsx
+++ b/excel/cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Program Files\Programs\Web Dev Related Stuff\Web Dev\Projects\EvaTion\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDAC64A7-B376-4037-A1C8-0A0A86E57BC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC86FF3B-FDD0-4518-92E9-4D3EF6715744}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -90,9 +90,6 @@
     <t>Industri farmasi dilaporkan memproduksi narkotika, setelah digrebek warga sekitar, pemiliknya setuju untuk datang ke Pengadilan.</t>
   </si>
   <si>
-    <t>Farmasi di sebuah desa tertangkap menyimpan ganja berbentuk tumbuhan, dan juga diketahui menanamnya tanpa izin, terhitung berat penyimpanan narkotikanya sebanyak 3,5 KG.</t>
-  </si>
-  <si>
     <t>Kasus ini diarahkan kepada farmasi. Seorang pecandu tertangkap dan mengakui tempat dimana Ia mendapat narkotikanya, pengedar narkotika itupun tertangkap dan diketahui bahwa sumber narkotika tersebut berasal dari sebuah farmasi ternama dan berizin memproduksi narkotika.</t>
   </si>
   <si>
@@ -232,6 +229,9 @@
   </si>
   <si>
     <t xml:space="preserve">Saat sedang melakukan pengecekan, sebuah narkotika yang berada pada tablet obat tanpa label ditemukan dalam sebuah farmasi. </t>
+  </si>
+  <si>
+    <t>Farmasi di sebuah desa tertangkap menyimpan ganja berbentuk tumbuhan, dan juga diketahui menanamnya tanpa izin, terhitung berat penyimpanan narkotikanya seberat 3,5 KG.</t>
   </si>
 </sst>
 </file>
@@ -633,8 +633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.8984375" defaultRowHeight="18"/>
@@ -678,7 +678,7 @@
         <v>18</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>10</v>
@@ -698,7 +698,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>11</v>
@@ -718,7 +718,7 @@
         <v>20</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>12</v>
@@ -735,10 +735,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>13</v>
@@ -755,10 +755,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>12</v>
@@ -775,10 +775,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>13</v>
@@ -795,10 +795,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>12</v>
@@ -815,10 +815,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>13</v>
@@ -835,10 +835,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>12</v>
@@ -858,7 +858,7 @@
         <v>6</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>13</v>
@@ -875,10 +875,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>12</v>
@@ -895,19 +895,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E13" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -915,19 +915,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E14" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -935,10 +935,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>13</v>
@@ -955,10 +955,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>12</v>
@@ -975,10 +975,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>13</v>
@@ -998,7 +998,7 @@
         <v>7</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>12</v>
@@ -1015,10 +1015,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>13</v>
@@ -1035,10 +1035,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>12</v>
@@ -1055,10 +1055,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>13</v>
@@ -1075,10 +1075,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>12</v>
@@ -1095,10 +1095,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>12</v>
@@ -1115,10 +1115,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>13</v>
@@ -1135,10 +1135,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>12</v>
@@ -1155,10 +1155,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>12</v>
@@ -1175,7 +1175,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>8</v>
@@ -1198,7 +1198,7 @@
         <v>9</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>14</v>
@@ -1215,10 +1215,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>15</v>
@@ -1235,10 +1235,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>16</v>
@@ -1255,10 +1255,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>17</v>

</xml_diff>